<commit_message>
Update form layout and clean views.py
</commit_message>
<xml_diff>
--- a/ChecklistSeiscomp/static/ChecklistSeiscomp/template.xlsx
+++ b/ChecklistSeiscomp/static/ChecklistSeiscomp/template.xlsx
@@ -2583,11 +2583,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="&quot;✔&quot;;;"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="&quot;✔&quot;;;"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -2729,10 +2729,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2744,9 +2744,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2755,21 +2754,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2806,18 +2790,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2830,21 +2821,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2877,7 +2877,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2889,175 +3057,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3557,6 +3557,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -3568,6 +3592,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3587,63 +3644,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -3657,10 +3657,10 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
@@ -3678,127 +3678,127 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="44">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="42">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="45">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="41">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="41">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="43">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="44">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="45">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="47">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="45">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="46">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="48">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="45">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="47">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="28" borderId="43">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="43">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="46">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="48">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3856,7 +3856,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3886,13 +3886,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
@@ -3920,26 +3920,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3951,7 +3951,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4362,8 +4362,8 @@
   </sheetPr>
   <dimension ref="A1:AC1140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="W187" sqref="W187:AB191"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="AD203" sqref="AD203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -42542,7 +42542,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.275590551181102" right="0.276" top="0.0930956848030019" bottom="0.551181102362205" header="0" footer="0"/>
-  <pageSetup paperSize="1" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="10000" scale="46" fitToHeight="0" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>